<commit_message>
fixed file excel template_user
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC28C763-6058-4D37-910B-1ACCB69A9FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F864C3B-4F78-4060-A0EF-50E1BA4F3D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56227778-A0C4-4A43-9963-92BBC3A3ED27}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +439,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>